<commit_message>
Criação do banco de dados
</commit_message>
<xml_diff>
--- a/modelo_db/modelo_projeto.xlsx
+++ b/modelo_db/modelo_projeto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\NOVA TURMA PORTAL TECH\HTML CSS\projeto_integrador_grupo_04\modelo_db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAB6AEAF-BF0E-4C0D-9500-60A84EC363D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1136A705-5340-4C32-8AE3-64BC2631D209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{871DA046-C98A-463A-84BA-0D7BF868AE6B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Clientes</t>
   </si>
@@ -86,15 +86,6 @@
     <t>cpf</t>
   </si>
   <si>
-    <t>id_end</t>
-  </si>
-  <si>
-    <t>id_login</t>
-  </si>
-  <si>
-    <t>cnpj_est</t>
-  </si>
-  <si>
     <t>cnpj_emp</t>
   </si>
   <si>
@@ -114,6 +105,15 @@
   </si>
   <si>
     <t>suv</t>
+  </si>
+  <si>
+    <t>placa</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>cnpj</t>
   </si>
 </sst>
 </file>
@@ -275,20 +275,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -388,6 +374,20 @@
         </bottom>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -402,13 +402,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{366B4068-E437-47E9-919A-8FB9D014DD10}" name="Tabela1" displayName="Tabela1" ref="A1:F13" totalsRowShown="0" dataDxfId="2">
-  <autoFilter ref="A1:F13" xr:uid="{366B4068-E437-47E9-919A-8FB9D014DD10}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{366B4068-E437-47E9-919A-8FB9D014DD10}" name="Tabela1" displayName="Tabela1" ref="A1:F14" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="A1:F14" xr:uid="{366B4068-E437-47E9-919A-8FB9D014DD10}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{572C0162-2BEF-4CA3-9958-F99B1D9704DA}" name="Clientes" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DFD63C22-BB06-4D38-8F79-6609FF448801}" name="Estacionamentos" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{75F54710-B5AF-41C7-AD04-9E98728F7634}" name="Login" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{0C14DB2B-1710-4BA5-BB37-C652BA366E00}" name="Empresas" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{572C0162-2BEF-4CA3-9958-F99B1D9704DA}" name="Clientes" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{DFD63C22-BB06-4D38-8F79-6609FF448801}" name="Estacionamentos" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{75F54710-B5AF-41C7-AD04-9E98728F7634}" name="Login" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{0C14DB2B-1710-4BA5-BB37-C652BA366E00}" name="Empresas" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{95C43AF8-C8F1-48AB-AF60-4C6BA10B1B7A}" name="Endereço" dataDxfId="1"/>
     <tableColumn id="6" xr3:uid="{BCEA273E-B99B-4993-AE1E-22427E098C22}" name="Veiculos" dataDxfId="0"/>
   </tableColumns>
@@ -713,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5304E7CF-12D1-4426-B8EF-D0FA8F4B347B}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="D2" sqref="D2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -745,107 +745,115 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>25</v>
+      <c r="F4" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -854,7 +862,9 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="3"/>
@@ -862,7 +872,9 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="3"/>
@@ -873,24 +885,32 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>